<commit_message>
Use 10 components in PCA
</commit_message>
<xml_diff>
--- a/data/A_rabiei_pathotypes_2013-2018.xlsx
+++ b/data/A_rabiei_pathotypes_2013-2018.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adido\OneDrive - Griffith University\Research\A_rabiei\A_rabiei_DArT\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s2978925\OneDrive - Griffith University\Research\A_rabiei\A_rabiei_DArT\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="6_{3475DE02-59FC-4BD9-89EC-5F3C309BE91A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{70A043BB-5248-4CBE-B8FB-A15BBF178932}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="6_{3475DE02-59FC-4BD9-89EC-5F3C309BE91A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{7AEE18E5-4640-4B51-8E80-B9AD59622A7E}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="4920" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29580" yWindow="780" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pathotyping" sheetId="7" r:id="rId1"/>
@@ -2528,7 +2528,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table5" displayName="Table5" ref="A1:L605" totalsRowShown="0">
-  <autoFilter ref="A1:L605" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+  <autoFilter ref="A1:L605" xr:uid="{00000000-0009-0000-0100-000004000000}">
+    <filterColumn colId="9">
+      <filters>
+        <filter val="2018"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A107:L206">
     <sortCondition ref="A1:A605"/>
   </sortState>
@@ -2848,12 +2854,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L605"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A407" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A589" workbookViewId="0">
       <selection activeCell="D426" sqref="D426"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
     <col min="2" max="2" width="23.140625" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" customWidth="1"/>
   </cols>
@@ -2896,7 +2903,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -2934,7 +2941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -2972,7 +2979,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -3010,7 +3017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -3048,7 +3055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -3086,7 +3093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -3124,7 +3131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -3162,7 +3169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -3200,7 +3207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -3238,7 +3245,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -3276,7 +3283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -3314,7 +3321,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -3352,7 +3359,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -3390,7 +3397,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>37</v>
       </c>
@@ -3428,7 +3435,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -3466,7 +3473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -3504,7 +3511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>40</v>
       </c>
@@ -3542,7 +3549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>42</v>
       </c>
@@ -3580,7 +3587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -3618,7 +3625,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>48</v>
       </c>
@@ -3656,7 +3663,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>49</v>
       </c>
@@ -3694,7 +3701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>51</v>
       </c>
@@ -3732,7 +3739,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>53</v>
       </c>
@@ -3770,7 +3777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>54</v>
       </c>
@@ -3808,7 +3815,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>55</v>
       </c>
@@ -3846,7 +3853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>56</v>
       </c>
@@ -3884,7 +3891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>57</v>
       </c>
@@ -3922,7 +3929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>58</v>
       </c>
@@ -3960,7 +3967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>59</v>
       </c>
@@ -3998,7 +4005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>60</v>
       </c>
@@ -4036,7 +4043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>61</v>
       </c>
@@ -4074,7 +4081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>63</v>
       </c>
@@ -4112,7 +4119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>64</v>
       </c>
@@ -4150,7 +4157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>65</v>
       </c>
@@ -4188,7 +4195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>66</v>
       </c>
@@ -4226,7 +4233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>67</v>
       </c>
@@ -4264,7 +4271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>68</v>
       </c>
@@ -4302,7 +4309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>69</v>
       </c>
@@ -4340,7 +4347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>70</v>
       </c>
@@ -4378,7 +4385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>71</v>
       </c>
@@ -4416,7 +4423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>72</v>
       </c>
@@ -4454,7 +4461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>73</v>
       </c>
@@ -4492,7 +4499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>74</v>
       </c>
@@ -4530,7 +4537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>75</v>
       </c>
@@ -4568,7 +4575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>76</v>
       </c>
@@ -4606,7 +4613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>77</v>
       </c>
@@ -4644,7 +4651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>80</v>
       </c>
@@ -4682,7 +4689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>83</v>
       </c>
@@ -4720,7 +4727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>86</v>
       </c>
@@ -4758,7 +4765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>89</v>
       </c>
@@ -4796,7 +4803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>90</v>
       </c>
@@ -4834,7 +4841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>94</v>
       </c>
@@ -4872,7 +4879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>95</v>
       </c>
@@ -4910,7 +4917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>97</v>
       </c>
@@ -4948,7 +4955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>98</v>
       </c>
@@ -4986,7 +4993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>99</v>
       </c>
@@ -5024,7 +5031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>100</v>
       </c>
@@ -5062,7 +5069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>101</v>
       </c>
@@ -5100,7 +5107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>102</v>
       </c>
@@ -5138,7 +5145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>103</v>
       </c>
@@ -5176,7 +5183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>104</v>
       </c>
@@ -5214,7 +5221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>105</v>
       </c>
@@ -5252,7 +5259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>106</v>
       </c>
@@ -5290,7 +5297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>107</v>
       </c>
@@ -5328,7 +5335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>108</v>
       </c>
@@ -5366,7 +5373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>109</v>
       </c>
@@ -5404,7 +5411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>110</v>
       </c>
@@ -5442,7 +5449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>111</v>
       </c>
@@ -5480,7 +5487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>112</v>
       </c>
@@ -5518,7 +5525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>113</v>
       </c>
@@ -5556,7 +5563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>114</v>
       </c>
@@ -5594,7 +5601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>115</v>
       </c>
@@ -5632,7 +5639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>116</v>
       </c>
@@ -5670,7 +5677,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>117</v>
       </c>
@@ -5708,7 +5715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>118</v>
       </c>
@@ -5746,7 +5753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>119</v>
       </c>
@@ -5784,7 +5791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>120</v>
       </c>
@@ -5822,7 +5829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>121</v>
       </c>
@@ -5860,7 +5867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>123</v>
       </c>
@@ -5898,7 +5905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>124</v>
       </c>
@@ -5936,7 +5943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>125</v>
       </c>
@@ -5974,7 +5981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>126</v>
       </c>
@@ -6012,7 +6019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>127</v>
       </c>
@@ -6050,7 +6057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>128</v>
       </c>
@@ -6088,7 +6095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>129</v>
       </c>
@@ -6126,7 +6133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>130</v>
       </c>
@@ -6164,7 +6171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>131</v>
       </c>
@@ -6202,7 +6209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>133</v>
       </c>
@@ -6240,7 +6247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>134</v>
       </c>
@@ -6278,7 +6285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>135</v>
       </c>
@@ -6316,7 +6323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>137</v>
       </c>
@@ -6354,7 +6361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>138</v>
       </c>
@@ -6392,7 +6399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>139</v>
       </c>
@@ -6430,7 +6437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>140</v>
       </c>
@@ -6468,7 +6475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>141</v>
       </c>
@@ -6506,7 +6513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>142</v>
       </c>
@@ -6544,7 +6551,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>143</v>
       </c>
@@ -6582,7 +6589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>144</v>
       </c>
@@ -6620,7 +6627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>145</v>
       </c>
@@ -6658,7 +6665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>146</v>
       </c>
@@ -6696,7 +6703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>147</v>
       </c>
@@ -6734,7 +6741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>148</v>
       </c>
@@ -6772,7 +6779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>149</v>
       </c>
@@ -6810,7 +6817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>150</v>
       </c>
@@ -6848,7 +6855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>151</v>
       </c>
@@ -6886,7 +6893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>268</v>
       </c>
@@ -6924,7 +6931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>270</v>
       </c>
@@ -6962,7 +6969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>266</v>
       </c>
@@ -7000,7 +7007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>267</v>
       </c>
@@ -7038,7 +7045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>164</v>
       </c>
@@ -7076,7 +7083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>166</v>
       </c>
@@ -7114,7 +7121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>247</v>
       </c>
@@ -7152,7 +7159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>248</v>
       </c>
@@ -7190,7 +7197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>249</v>
       </c>
@@ -7228,7 +7235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>250</v>
       </c>
@@ -7266,7 +7273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>251</v>
       </c>
@@ -7304,7 +7311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>252</v>
       </c>
@@ -7342,7 +7349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>254</v>
       </c>
@@ -7380,7 +7387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>256</v>
       </c>
@@ -7418,7 +7425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>257</v>
       </c>
@@ -7456,7 +7463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>258</v>
       </c>
@@ -7494,7 +7501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>259</v>
       </c>
@@ -7532,7 +7539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>260</v>
       </c>
@@ -7570,7 +7577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>261</v>
       </c>
@@ -7608,7 +7615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>262</v>
       </c>
@@ -7646,7 +7653,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>263</v>
       </c>
@@ -7684,7 +7691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>264</v>
       </c>
@@ -7722,7 +7729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>161</v>
       </c>
@@ -7760,7 +7767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>271</v>
       </c>
@@ -7798,7 +7805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>273</v>
       </c>
@@ -7836,7 +7843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>177</v>
       </c>
@@ -7874,7 +7881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>178</v>
       </c>
@@ -7912,7 +7919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>179</v>
       </c>
@@ -7950,7 +7957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>275</v>
       </c>
@@ -7988,7 +7995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>167</v>
       </c>
@@ -8026,7 +8033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>180</v>
       </c>
@@ -8064,7 +8071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>182</v>
       </c>
@@ -8102,7 +8109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>183</v>
       </c>
@@ -8140,7 +8147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>184</v>
       </c>
@@ -8178,7 +8185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>185</v>
       </c>
@@ -8216,7 +8223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>186</v>
       </c>
@@ -8254,7 +8261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>187</v>
       </c>
@@ -8292,7 +8299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>188</v>
       </c>
@@ -8330,7 +8337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>152</v>
       </c>
@@ -8368,7 +8375,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>189</v>
       </c>
@@ -8406,7 +8413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>190</v>
       </c>
@@ -8444,7 +8451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>154</v>
       </c>
@@ -8482,7 +8489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>191</v>
       </c>
@@ -8520,7 +8527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>155</v>
       </c>
@@ -8558,7 +8565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>156</v>
       </c>
@@ -8596,7 +8603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>192</v>
       </c>
@@ -8634,7 +8641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>193</v>
       </c>
@@ -8672,7 +8679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>194</v>
       </c>
@@ -8710,7 +8717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>195</v>
       </c>
@@ -8748,7 +8755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>196</v>
       </c>
@@ -8786,7 +8793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>197</v>
       </c>
@@ -8824,7 +8831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>198</v>
       </c>
@@ -8862,7 +8869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>199</v>
       </c>
@@ -8900,7 +8907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>157</v>
       </c>
@@ -8938,7 +8945,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>200</v>
       </c>
@@ -8976,7 +8983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>158</v>
       </c>
@@ -9014,7 +9021,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>201</v>
       </c>
@@ -9052,7 +9059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>202</v>
       </c>
@@ -9090,7 +9097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>203</v>
       </c>
@@ -9128,7 +9135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>159</v>
       </c>
@@ -9166,7 +9173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>160</v>
       </c>
@@ -9204,7 +9211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>204</v>
       </c>
@@ -9242,7 +9249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>205</v>
       </c>
@@ -9280,7 +9287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>206</v>
       </c>
@@ -9318,7 +9325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>207</v>
       </c>
@@ -9356,7 +9363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>208</v>
       </c>
@@ -9394,7 +9401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>170</v>
       </c>
@@ -9432,7 +9439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>172</v>
       </c>
@@ -9470,7 +9477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>173</v>
       </c>
@@ -9508,7 +9515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>174</v>
       </c>
@@ -9546,7 +9553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>176</v>
       </c>
@@ -9584,7 +9591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>209</v>
       </c>
@@ -9622,7 +9629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>210</v>
       </c>
@@ -9660,7 +9667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>212</v>
       </c>
@@ -9698,7 +9705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>213</v>
       </c>
@@ -9736,7 +9743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>214</v>
       </c>
@@ -9774,7 +9781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>215</v>
       </c>
@@ -9812,7 +9819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>217</v>
       </c>
@@ -9850,7 +9857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>218</v>
       </c>
@@ -9888,7 +9895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>221</v>
       </c>
@@ -9926,7 +9933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>222</v>
       </c>
@@ -9964,7 +9971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>224</v>
       </c>
@@ -10002,7 +10009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>225</v>
       </c>
@@ -10040,7 +10047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>226</v>
       </c>
@@ -10078,7 +10085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>227</v>
       </c>
@@ -10116,7 +10123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>228</v>
       </c>
@@ -10154,7 +10161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>229</v>
       </c>
@@ -10192,7 +10199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>231</v>
       </c>
@@ -10230,7 +10237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>233</v>
       </c>
@@ -10268,7 +10275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>234</v>
       </c>
@@ -10306,7 +10313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>235</v>
       </c>
@@ -10344,7 +10351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>236</v>
       </c>
@@ -10382,7 +10389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>238</v>
       </c>
@@ -10420,7 +10427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>239</v>
       </c>
@@ -10458,7 +10465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>240</v>
       </c>
@@ -10496,7 +10503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>241</v>
       </c>
@@ -10534,7 +10541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>242</v>
       </c>
@@ -10572,7 +10579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>243</v>
       </c>
@@ -10610,7 +10617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>245</v>
       </c>
@@ -10648,7 +10655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>246</v>
       </c>
@@ -10686,7 +10693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>278</v>
       </c>
@@ -10724,7 +10731,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="208" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>280</v>
       </c>
@@ -10762,7 +10769,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="209" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>281</v>
       </c>
@@ -10800,7 +10807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>282</v>
       </c>
@@ -10838,7 +10845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>283</v>
       </c>
@@ -10876,7 +10883,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="212" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>284</v>
       </c>
@@ -10914,7 +10921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>285</v>
       </c>
@@ -10952,7 +10959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>286</v>
       </c>
@@ -10990,7 +10997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>287</v>
       </c>
@@ -11028,7 +11035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="216" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>288</v>
       </c>
@@ -11066,7 +11073,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="217" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>289</v>
       </c>
@@ -11104,7 +11111,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="218" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>290</v>
       </c>
@@ -11142,7 +11149,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="219" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>291</v>
       </c>
@@ -11180,7 +11187,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="220" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>292</v>
       </c>
@@ -11218,7 +11225,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="221" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>293</v>
       </c>
@@ -11256,7 +11263,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="222" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>294</v>
       </c>
@@ -11294,7 +11301,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="223" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>295</v>
       </c>
@@ -11332,7 +11339,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="224" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>296</v>
       </c>
@@ -11370,7 +11377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="225" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>298</v>
       </c>
@@ -11408,7 +11415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>299</v>
       </c>
@@ -11446,7 +11453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>300</v>
       </c>
@@ -11484,7 +11491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>301</v>
       </c>
@@ -11522,7 +11529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>302</v>
       </c>
@@ -11560,7 +11567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>303</v>
       </c>
@@ -11598,7 +11605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>306</v>
       </c>
@@ -11636,7 +11643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>307</v>
       </c>
@@ -11674,7 +11681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>308</v>
       </c>
@@ -11712,7 +11719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>309</v>
       </c>
@@ -11750,7 +11757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>310</v>
       </c>
@@ -11788,7 +11795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>312</v>
       </c>
@@ -11826,7 +11833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>313</v>
       </c>
@@ -11864,7 +11871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>314</v>
       </c>
@@ -11902,7 +11909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>315</v>
       </c>
@@ -11940,7 +11947,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="240" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>805</v>
       </c>
@@ -11978,7 +11985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>806</v>
       </c>
@@ -12016,7 +12023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="242" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>807</v>
       </c>
@@ -12054,7 +12061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="243" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>808</v>
       </c>
@@ -12092,7 +12099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="244" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>809</v>
       </c>
@@ -12130,7 +12137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="245" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>810</v>
       </c>
@@ -12168,7 +12175,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="246" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>811</v>
       </c>
@@ -12206,7 +12213,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="247" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>812</v>
       </c>
@@ -12244,7 +12251,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="248" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>813</v>
       </c>
@@ -12282,7 +12289,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="249" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>814</v>
       </c>
@@ -12320,7 +12327,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="250" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>815</v>
       </c>
@@ -12358,7 +12365,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="251" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>816</v>
       </c>
@@ -12396,7 +12403,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="252" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>317</v>
       </c>
@@ -12434,7 +12441,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="253" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>318</v>
       </c>
@@ -12472,7 +12479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>320</v>
       </c>
@@ -12510,7 +12517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>321</v>
       </c>
@@ -12548,7 +12555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="256" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>323</v>
       </c>
@@ -12586,7 +12593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="257" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>324</v>
       </c>
@@ -12624,7 +12631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="258" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>325</v>
       </c>
@@ -12662,7 +12669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="259" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>326</v>
       </c>
@@ -12700,7 +12707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="260" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>327</v>
       </c>
@@ -12738,7 +12745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>329</v>
       </c>
@@ -12776,7 +12783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>330</v>
       </c>
@@ -12814,7 +12821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="263" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>331</v>
       </c>
@@ -12852,7 +12859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="264" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>332</v>
       </c>
@@ -12890,7 +12897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>334</v>
       </c>
@@ -12928,7 +12935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>335</v>
       </c>
@@ -12966,7 +12973,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>336</v>
       </c>
@@ -13004,7 +13011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="268" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>338</v>
       </c>
@@ -13042,7 +13049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="269" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>339</v>
       </c>
@@ -13080,7 +13087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>341</v>
       </c>
@@ -13118,7 +13125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="271" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>343</v>
       </c>
@@ -13156,7 +13163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="272" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>344</v>
       </c>
@@ -13194,7 +13201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>345</v>
       </c>
@@ -13232,7 +13239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>346</v>
       </c>
@@ -13270,7 +13277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="275" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>348</v>
       </c>
@@ -13308,7 +13315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="276" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>350</v>
       </c>
@@ -13346,7 +13353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="277" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>351</v>
       </c>
@@ -13384,7 +13391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="278" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>352</v>
       </c>
@@ -13422,7 +13429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>353</v>
       </c>
@@ -13460,7 +13467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>355</v>
       </c>
@@ -13498,7 +13505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="281" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>356</v>
       </c>
@@ -13536,7 +13543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>357</v>
       </c>
@@ -13574,7 +13581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>358</v>
       </c>
@@ -13612,7 +13619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>360</v>
       </c>
@@ -13650,7 +13657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>361</v>
       </c>
@@ -13688,7 +13695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>362</v>
       </c>
@@ -13726,7 +13733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="287" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>363</v>
       </c>
@@ -13764,7 +13771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>364</v>
       </c>
@@ -13802,7 +13809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="289" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>366</v>
       </c>
@@ -13840,7 +13847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="290" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>367</v>
       </c>
@@ -13878,7 +13885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="291" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>368</v>
       </c>
@@ -13916,7 +13923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="292" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>369</v>
       </c>
@@ -13954,7 +13961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>370</v>
       </c>
@@ -13992,7 +13999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>372</v>
       </c>
@@ -14030,7 +14037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>373</v>
       </c>
@@ -14068,7 +14075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>374</v>
       </c>
@@ -14106,7 +14113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>375</v>
       </c>
@@ -14144,7 +14151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>376</v>
       </c>
@@ -14182,7 +14189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>378</v>
       </c>
@@ -14220,7 +14227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>379</v>
       </c>
@@ -14258,7 +14265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>380</v>
       </c>
@@ -14296,7 +14303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="302" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>381</v>
       </c>
@@ -14334,7 +14341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="303" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>382</v>
       </c>
@@ -14372,7 +14379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="304" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>384</v>
       </c>
@@ -14410,7 +14417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="305" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>385</v>
       </c>
@@ -14448,7 +14455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="306" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>386</v>
       </c>
@@ -14486,7 +14493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="307" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>387</v>
       </c>
@@ -14524,7 +14531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="308" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>388</v>
       </c>
@@ -14562,7 +14569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="309" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>390</v>
       </c>
@@ -14600,7 +14607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="310" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>391</v>
       </c>
@@ -14638,7 +14645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="311" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>392</v>
       </c>
@@ -14676,7 +14683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="312" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>393</v>
       </c>
@@ -14714,7 +14721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="313" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>394</v>
       </c>
@@ -14752,7 +14759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="314" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>395</v>
       </c>
@@ -14790,7 +14797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="315" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>396</v>
       </c>
@@ -14828,7 +14835,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="316" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>397</v>
       </c>
@@ -14866,7 +14873,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="317" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>398</v>
       </c>
@@ -14904,7 +14911,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="318" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>399</v>
       </c>
@@ -14942,7 +14949,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="319" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>400</v>
       </c>
@@ -14980,7 +14987,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="320" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>401</v>
       </c>
@@ -15018,7 +15025,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="321" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>402</v>
       </c>
@@ -15056,7 +15063,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="322" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>403</v>
       </c>
@@ -15094,7 +15101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="323" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>405</v>
       </c>
@@ -15132,7 +15139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="324" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>406</v>
       </c>
@@ -15170,7 +15177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="325" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>407</v>
       </c>
@@ -15208,7 +15215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="326" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>408</v>
       </c>
@@ -15246,7 +15253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="327" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>409</v>
       </c>
@@ -15284,7 +15291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="328" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>410</v>
       </c>
@@ -15322,7 +15329,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="329" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>411</v>
       </c>
@@ -15360,7 +15367,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="330" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>412</v>
       </c>
@@ -15398,7 +15405,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="331" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>413</v>
       </c>
@@ -15436,7 +15443,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="332" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>414</v>
       </c>
@@ -15474,7 +15481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="333" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>415</v>
       </c>
@@ -15512,7 +15519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="334" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>416</v>
       </c>
@@ -15550,7 +15557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="335" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>417</v>
       </c>
@@ -15588,7 +15595,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="336" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>418</v>
       </c>
@@ -15626,7 +15633,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="337" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>419</v>
       </c>
@@ -15664,7 +15671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="338" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>422</v>
       </c>
@@ -15702,7 +15709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="339" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>423</v>
       </c>
@@ -15740,7 +15747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="340" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>424</v>
       </c>
@@ -15778,7 +15785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="341" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>425</v>
       </c>
@@ -15816,7 +15823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="342" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>426</v>
       </c>
@@ -15854,7 +15861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="343" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>427</v>
       </c>
@@ -15892,7 +15899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="344" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>428</v>
       </c>
@@ -15930,7 +15937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="345" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>429</v>
       </c>
@@ -15968,7 +15975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="346" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>430</v>
       </c>
@@ -16006,7 +16013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="347" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>431</v>
       </c>
@@ -16044,7 +16051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="348" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>433</v>
       </c>
@@ -16082,7 +16089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="349" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>434</v>
       </c>
@@ -16120,7 +16127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="350" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>435</v>
       </c>
@@ -16158,7 +16165,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="351" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>436</v>
       </c>
@@ -16196,7 +16203,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="352" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>438</v>
       </c>
@@ -16234,7 +16241,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="353" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>440</v>
       </c>
@@ -16272,7 +16279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="354" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>442</v>
       </c>
@@ -16310,7 +16317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="355" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>444</v>
       </c>
@@ -16348,7 +16355,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="356" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>446</v>
       </c>
@@ -16386,7 +16393,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="357" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>448</v>
       </c>
@@ -16424,7 +16431,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="358" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
         <v>449</v>
       </c>
@@ -16462,7 +16469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="359" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>451</v>
       </c>
@@ -16500,7 +16507,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="360" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>452</v>
       </c>
@@ -16538,7 +16545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="361" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>454</v>
       </c>
@@ -16576,7 +16583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="362" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>455</v>
       </c>
@@ -16614,7 +16621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="363" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
         <v>458</v>
       </c>
@@ -16652,7 +16659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="364" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>459</v>
       </c>
@@ -16690,7 +16697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="365" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>460</v>
       </c>
@@ -16728,7 +16735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="366" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
         <v>461</v>
       </c>
@@ -16766,7 +16773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="367" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
         <v>462</v>
       </c>
@@ -16804,7 +16811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="368" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
         <v>463</v>
       </c>
@@ -16842,7 +16849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="369" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
         <v>464</v>
       </c>
@@ -16880,7 +16887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="370" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
         <v>465</v>
       </c>
@@ -16918,7 +16925,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="371" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
         <v>466</v>
       </c>
@@ -16956,7 +16963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="372" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
         <v>467</v>
       </c>
@@ -16994,7 +17001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="373" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
         <v>469</v>
       </c>
@@ -17032,7 +17039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="374" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
         <v>470</v>
       </c>
@@ -17070,7 +17077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="375" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
         <v>471</v>
       </c>
@@ -17108,7 +17115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="376" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
         <v>472</v>
       </c>
@@ -17146,7 +17153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="377" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
         <v>474</v>
       </c>
@@ -17184,7 +17191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="378" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
         <v>475</v>
       </c>
@@ -17222,7 +17229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="379" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
         <v>476</v>
       </c>
@@ -17260,7 +17267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="380" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
         <v>478</v>
       </c>
@@ -17298,7 +17305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="381" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
         <v>479</v>
       </c>
@@ -17336,7 +17343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="382" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
         <v>480</v>
       </c>
@@ -17374,7 +17381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="383" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
         <v>481</v>
       </c>
@@ -17412,7 +17419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="384" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
         <v>482</v>
       </c>
@@ -17450,7 +17457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="385" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
         <v>483</v>
       </c>
@@ -17488,7 +17495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="386" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
         <v>484</v>
       </c>
@@ -17526,7 +17533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="387" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
         <v>485</v>
       </c>
@@ -17564,7 +17571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="388" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
         <v>486</v>
       </c>
@@ -17602,7 +17609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="389" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
         <v>487</v>
       </c>
@@ -17640,7 +17647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="390" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
         <v>489</v>
       </c>
@@ -17678,7 +17685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="391" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
         <v>490</v>
       </c>
@@ -17716,7 +17723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="392" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
         <v>491</v>
       </c>
@@ -17754,7 +17761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="393" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
         <v>493</v>
       </c>
@@ -17792,7 +17799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="394" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
         <v>494</v>
       </c>
@@ -17830,7 +17837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="395" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
         <v>495</v>
       </c>
@@ -17868,7 +17875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="396" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
         <v>496</v>
       </c>
@@ -17906,7 +17913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="397" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
         <v>497</v>
       </c>
@@ -17944,7 +17951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="398" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
         <v>498</v>
       </c>
@@ -17982,7 +17989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="399" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
         <v>500</v>
       </c>
@@ -18020,7 +18027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="400" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
         <v>501</v>
       </c>
@@ -18058,7 +18065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="401" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="401" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
         <v>502</v>
       </c>
@@ -18096,7 +18103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="402" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
         <v>503</v>
       </c>
@@ -18134,7 +18141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="403" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
         <v>504</v>
       </c>
@@ -18172,7 +18179,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="404" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
         <v>506</v>
       </c>
@@ -18210,7 +18217,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="405" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
         <v>507</v>
       </c>
@@ -18248,7 +18255,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="406" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="406" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
         <v>508</v>
       </c>
@@ -18286,7 +18293,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="407" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
         <v>509</v>
       </c>
@@ -18324,7 +18331,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="408" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
         <v>510</v>
       </c>
@@ -18362,7 +18369,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="409" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
         <v>511</v>
       </c>
@@ -18400,7 +18407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="410" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
         <v>512</v>
       </c>
@@ -18438,7 +18445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="411" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
         <v>514</v>
       </c>
@@ -18476,7 +18483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="412" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
         <v>515</v>
       </c>
@@ -18514,7 +18521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="413" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
         <v>516</v>
       </c>
@@ -18552,7 +18559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="414" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
         <v>517</v>
       </c>
@@ -18590,7 +18597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="415" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
         <v>518</v>
       </c>
@@ -18628,7 +18635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="416" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
         <v>519</v>
       </c>
@@ -18666,7 +18673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="417" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
         <v>520</v>
       </c>
@@ -18704,7 +18711,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="418" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
         <v>522</v>
       </c>
@@ -18742,7 +18749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="419" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="419" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
         <v>523</v>
       </c>
@@ -18780,7 +18787,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="420" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
         <v>524</v>
       </c>
@@ -18818,7 +18825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="421" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
         <v>525</v>
       </c>
@@ -18856,7 +18863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="422" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
         <v>526</v>
       </c>
@@ -18894,7 +18901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="423" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
         <v>527</v>
       </c>
@@ -18932,7 +18939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="424" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
         <v>528</v>
       </c>
@@ -18970,7 +18977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="425" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
         <v>529</v>
       </c>
@@ -19008,7 +19015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="426" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
         <v>531</v>
       </c>
@@ -19046,7 +19053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="427" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
         <v>533</v>
       </c>
@@ -19084,7 +19091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="428" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
         <v>534</v>
       </c>
@@ -19122,7 +19129,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="429" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
         <v>536</v>
       </c>
@@ -19160,7 +19167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="430" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
         <v>538</v>
       </c>
@@ -19198,7 +19205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="431" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
         <v>539</v>
       </c>
@@ -19236,7 +19243,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="432" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
         <v>541</v>
       </c>
@@ -19274,7 +19281,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="433" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
         <v>542</v>
       </c>
@@ -19312,7 +19319,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="434" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
         <v>543</v>
       </c>
@@ -19350,7 +19357,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="435" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
         <v>545</v>
       </c>
@@ -19388,7 +19395,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="436" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
         <v>546</v>
       </c>
@@ -19426,7 +19433,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="437" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
         <v>547</v>
       </c>
@@ -19464,7 +19471,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="438" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
         <v>549</v>
       </c>
@@ -19502,7 +19509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="439" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
         <v>550</v>
       </c>
@@ -19540,7 +19547,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="440" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
         <v>551</v>
       </c>
@@ -19578,7 +19585,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="441" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
         <v>553</v>
       </c>
@@ -19616,7 +19623,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="442" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
         <v>554</v>
       </c>
@@ -19654,7 +19661,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="443" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
         <v>555</v>
       </c>
@@ -19692,7 +19699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="444" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
         <v>557</v>
       </c>
@@ -19730,7 +19737,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="445" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
         <v>558</v>
       </c>
@@ -19768,7 +19775,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="446" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
         <v>559</v>
       </c>
@@ -19806,7 +19813,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="447" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A447" t="s">
         <v>560</v>
       </c>
@@ -19844,7 +19851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="448" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
         <v>563</v>
       </c>
@@ -19882,7 +19889,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="449" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
         <v>564</v>
       </c>
@@ -19920,7 +19927,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="450" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A450" t="s">
         <v>565</v>
       </c>
@@ -19958,7 +19965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="451" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A451" t="s">
         <v>792</v>
       </c>
@@ -19996,7 +20003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="452" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A452" t="s">
         <v>793</v>
       </c>
@@ -20034,7 +20041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="453" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A453" t="s">
         <v>794</v>
       </c>
@@ -20072,7 +20079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="454" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A454" t="s">
         <v>795</v>
       </c>
@@ -20110,7 +20117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="455" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A455" t="s">
         <v>796</v>
       </c>
@@ -20148,7 +20155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="456" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A456" t="s">
         <v>797</v>
       </c>
@@ -20186,7 +20193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="457" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A457" t="s">
         <v>798</v>
       </c>
@@ -20224,7 +20231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="458" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A458" t="s">
         <v>799</v>
       </c>
@@ -20262,7 +20269,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="459" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A459" t="s">
         <v>800</v>
       </c>
@@ -20300,7 +20307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="460" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A460" t="s">
         <v>801</v>
       </c>
@@ -20338,7 +20345,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="461" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A461" t="s">
         <v>802</v>
       </c>
@@ -20376,7 +20383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="462" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A462" t="s">
         <v>803</v>
       </c>
@@ -20414,7 +20421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="463" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A463" t="s">
         <v>804</v>
       </c>
@@ -20452,7 +20459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="464" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A464" t="s">
         <v>568</v>
       </c>
@@ -20490,7 +20497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="465" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A465" t="s">
         <v>571</v>
       </c>
@@ -20528,7 +20535,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="466" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A466" t="s">
         <v>572</v>
       </c>
@@ -20566,7 +20573,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="467" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A467" t="s">
         <v>573</v>
       </c>
@@ -20604,7 +20611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="468" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A468" t="s">
         <v>574</v>
       </c>
@@ -20642,7 +20649,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="469" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A469" t="s">
         <v>575</v>
       </c>
@@ -20680,7 +20687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="470" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A470" t="s">
         <v>576</v>
       </c>
@@ -20718,7 +20725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="471" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A471" t="s">
         <v>577</v>
       </c>
@@ -20756,7 +20763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="472" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A472" t="s">
         <v>579</v>
       </c>
@@ -20794,7 +20801,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="473" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A473" t="s">
         <v>581</v>
       </c>
@@ -20832,7 +20839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="474" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A474" t="s">
         <v>583</v>
       </c>
@@ -20870,7 +20877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="475" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A475" t="s">
         <v>584</v>
       </c>
@@ -20908,7 +20915,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="476" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A476" t="s">
         <v>585</v>
       </c>
@@ -20946,7 +20953,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="477" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A477" t="s">
         <v>586</v>
       </c>
@@ -20984,7 +20991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="478" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A478" t="s">
         <v>588</v>
       </c>
@@ -21022,7 +21029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="479" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A479" t="s">
         <v>590</v>
       </c>
@@ -21060,7 +21067,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="480" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A480" t="s">
         <v>591</v>
       </c>
@@ -21098,7 +21105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="481" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A481" t="s">
         <v>592</v>
       </c>
@@ -21136,7 +21143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="482" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="482" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A482" t="s">
         <v>593</v>
       </c>
@@ -21174,7 +21181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="483" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="483" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A483" t="s">
         <v>595</v>
       </c>
@@ -21212,7 +21219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="484" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A484" t="s">
         <v>596</v>
       </c>
@@ -21250,7 +21257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="485" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="485" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A485" t="s">
         <v>597</v>
       </c>
@@ -21288,7 +21295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="486" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A486" t="s">
         <v>598</v>
       </c>
@@ -21326,7 +21333,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="487" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="487" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A487" t="s">
         <v>599</v>
       </c>
@@ -21364,7 +21371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="488" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="488" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A488" t="s">
         <v>601</v>
       </c>
@@ -21402,7 +21409,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="489" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="489" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A489" t="s">
         <v>603</v>
       </c>
@@ -21440,7 +21447,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="490" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="490" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A490" t="s">
         <v>604</v>
       </c>
@@ -21478,7 +21485,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="491" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="491" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A491" t="s">
         <v>605</v>
       </c>
@@ -21516,7 +21523,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="492" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A492" t="s">
         <v>606</v>
       </c>
@@ -21554,7 +21561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="493" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="493" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A493" t="s">
         <v>607</v>
       </c>
@@ -21592,7 +21599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="494" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="494" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A494" t="s">
         <v>608</v>
       </c>
@@ -21630,7 +21637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="495" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="495" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A495" t="s">
         <v>609</v>
       </c>
@@ -21668,7 +21675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="496" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="496" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A496" t="s">
         <v>610</v>
       </c>
@@ -21706,7 +21713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="497" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="497" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A497" t="s">
         <v>611</v>
       </c>
@@ -21744,7 +21751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="498" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="498" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A498" t="s">
         <v>612</v>
       </c>
@@ -21782,7 +21789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="499" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="499" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A499" t="s">
         <v>614</v>
       </c>
@@ -21820,7 +21827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="500" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="500" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A500" t="s">
         <v>615</v>
       </c>
@@ -21858,7 +21865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="501" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="501" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A501" t="s">
         <v>616</v>
       </c>
@@ -21896,7 +21903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="502" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="502" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A502" t="s">
         <v>617</v>
       </c>
@@ -21934,7 +21941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="503" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="503" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A503" t="s">
         <v>618</v>
       </c>
@@ -21972,7 +21979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="504" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="504" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A504" t="s">
         <v>619</v>
       </c>
@@ -22010,7 +22017,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="505" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="505" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A505" t="s">
         <v>620</v>
       </c>
@@ -22048,7 +22055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="506" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="506" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A506" t="s">
         <v>621</v>
       </c>
@@ -22086,7 +22093,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="507" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="507" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A507" t="s">
         <v>622</v>
       </c>
@@ -22124,7 +22131,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="508" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="508" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A508" t="s">
         <v>623</v>
       </c>
@@ -22162,7 +22169,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="509" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="509" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A509" t="s">
         <v>624</v>
       </c>
@@ -22200,7 +22207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="510" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="510" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A510" t="s">
         <v>625</v>
       </c>
@@ -26655,6 +26662,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010038EC5152544FA941B2FCF6FC911C1211" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c65ce02839d668ca9eba218866de938">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f38ef60c-44b8-4b3e-b84e-3f774f47ec01" xmlns:ns4="77420ce7-ad61-40a5-b28d-42d2f2a680a0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f5d8e21d1066e7b0b912dd2073999255" ns3:_="" ns4:_="">
     <xsd:import namespace="f38ef60c-44b8-4b3e-b84e-3f774f47ec01"/>
@@ -26863,15 +26879,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -26879,6 +26886,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C120FF30-B511-4131-BD85-85594DEF917C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{314AA4AE-DDAA-446D-8180-DBC3DDACA6AA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -26893,14 +26908,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C120FF30-B511-4131-BD85-85594DEF917C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>